<commit_message>
Added test comparison images
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlada\Documents\Git\vu-isi-student-results\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlada\Documents\Git\VU ISI\OP\vu-isi-student-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="17">
   <si>
     <t>10^3</t>
   </si>
@@ -65,10 +65,16 @@
     <t>Strategy No. 2</t>
   </si>
   <si>
-    <t>optimised vector</t>
+    <t>~0</t>
   </si>
   <si>
-    <t>~0</t>
+    <t>vector_o</t>
+  </si>
+  <si>
+    <t>vector (1)</t>
+  </si>
+  <si>
+    <t>vector (2)</t>
   </si>
 </sst>
 </file>
@@ -104,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -112,6 +118,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,75 +412,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="O5" s="2" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="O5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -564,7 +582,7 @@
         <v>126.6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -620,7 +638,7 @@
         <v>117.4</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -676,58 +694,58 @@
         <v>103.77</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="H15" s="2" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="H15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="O15" s="2" t="s">
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="O15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -815,22 +833,22 @@
         <v>5</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -886,7 +904,7 @@
         <v>97.46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -927,7 +945,7 @@
         <v>7</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q20">
         <v>0.52</v>
@@ -942,33 +960,33 @@
         <v>534.75</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="H23" s="2" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="H23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="O23" s="2" t="s">
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="O23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,75 +1033,706 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B26">
         <v>0.04</v>
       </c>
       <c r="C26">
-        <v>0.43</v>
+        <v>0.45</v>
       </c>
       <c r="D26">
-        <v>4.38</v>
+        <v>4.28</v>
       </c>
       <c r="E26">
-        <v>44.26</v>
+        <v>43.4</v>
       </c>
       <c r="F26">
-        <v>515.02</v>
+        <v>507.99</v>
       </c>
       <c r="H26" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="I26">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="J26">
-        <v>1.0900000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="K26">
-        <v>9.9700000000000006</v>
+        <v>10.944000000000001</v>
       </c>
       <c r="L26">
-        <v>105.95</v>
+        <v>104.15</v>
       </c>
       <c r="M26">
-        <v>1178.97</v>
+        <v>1109.1600000000001</v>
       </c>
       <c r="O26" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="P26">
         <v>0.01</v>
       </c>
       <c r="Q26">
+        <v>0.12</v>
+      </c>
+      <c r="R26">
+        <v>1.01</v>
+      </c>
+      <c r="S26">
+        <v>10.51</v>
+      </c>
+      <c r="T26">
+        <v>126.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>0.04</v>
+      </c>
+      <c r="C27">
+        <v>0.42</v>
+      </c>
+      <c r="D27">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="E27">
+        <v>43.56</v>
+      </c>
+      <c r="F27">
+        <v>511.5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>0.13</v>
+      </c>
+      <c r="J27">
+        <v>1.02</v>
+      </c>
+      <c r="K27">
+        <v>10.46</v>
+      </c>
+      <c r="L27">
+        <v>103.11</v>
+      </c>
+      <c r="M27">
+        <v>1145.02</v>
+      </c>
+      <c r="O27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>0.04</v>
+      </c>
+      <c r="C28">
+        <v>0.43</v>
+      </c>
+      <c r="D28">
+        <v>4.38</v>
+      </c>
+      <c r="E28">
+        <v>44.26</v>
+      </c>
+      <c r="F28">
+        <v>515.02</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28">
+        <v>0.15</v>
+      </c>
+      <c r="J28">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K28">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="L28">
+        <v>105.95</v>
+      </c>
+      <c r="M28">
+        <v>1178.97</v>
+      </c>
+      <c r="O28" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28">
+        <v>0.01</v>
+      </c>
+      <c r="Q28">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="R26">
+      <c r="R28">
         <v>0.79</v>
       </c>
-      <c r="S26">
+      <c r="S28">
         <v>7</v>
       </c>
-      <c r="T26">
+      <c r="T28">
         <v>79.55</v>
       </c>
     </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="M32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="Y32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="4"/>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="7"/>
+      <c r="J34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="7"/>
+      <c r="N34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O34" s="7"/>
+      <c r="P34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" s="7"/>
+      <c r="T34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U34" s="7"/>
+      <c r="V34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="W34" s="7"/>
+      <c r="Z34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI34" s="7"/>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B35" s="8">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8">
+        <v>2</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1</v>
+      </c>
+      <c r="E35" s="8">
+        <v>2</v>
+      </c>
+      <c r="F35" s="8">
+        <v>1</v>
+      </c>
+      <c r="G35" s="8">
+        <v>2</v>
+      </c>
+      <c r="H35" s="8">
+        <v>1</v>
+      </c>
+      <c r="I35" s="8">
+        <v>2</v>
+      </c>
+      <c r="J35" s="8">
+        <v>1</v>
+      </c>
+      <c r="K35" s="8">
+        <v>2</v>
+      </c>
+      <c r="N35" s="8">
+        <v>1</v>
+      </c>
+      <c r="O35" s="8">
+        <v>2</v>
+      </c>
+      <c r="P35" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>2</v>
+      </c>
+      <c r="R35" s="8">
+        <v>1</v>
+      </c>
+      <c r="S35" s="8">
+        <v>2</v>
+      </c>
+      <c r="T35" s="8">
+        <v>1</v>
+      </c>
+      <c r="U35" s="8">
+        <v>2</v>
+      </c>
+      <c r="V35" s="8">
+        <v>1</v>
+      </c>
+      <c r="W35" s="8">
+        <v>2</v>
+      </c>
+      <c r="Z35" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="8">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD35" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF35" s="8">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="8">
+        <v>2</v>
+      </c>
+      <c r="AH35" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>0.04</v>
+      </c>
+      <c r="C36">
+        <v>0.04</v>
+      </c>
+      <c r="D36">
+        <v>0.45</v>
+      </c>
+      <c r="E36">
+        <v>0.42</v>
+      </c>
+      <c r="F36">
+        <v>4.28</v>
+      </c>
+      <c r="G36">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="H36">
+        <v>43.4</v>
+      </c>
+      <c r="I36">
+        <v>43.56</v>
+      </c>
+      <c r="J36">
+        <v>507.99</v>
+      </c>
+      <c r="K36">
+        <v>511.5</v>
+      </c>
+      <c r="M36" t="s">
+        <v>5</v>
+      </c>
+      <c r="N36">
+        <v>0.13</v>
+      </c>
+      <c r="O36">
+        <v>0.13</v>
+      </c>
+      <c r="P36">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q36">
+        <v>1.02</v>
+      </c>
+      <c r="R36">
+        <v>10.944000000000001</v>
+      </c>
+      <c r="S36">
+        <v>10.46</v>
+      </c>
+      <c r="T36">
+        <v>104.15</v>
+      </c>
+      <c r="U36">
+        <v>103.11</v>
+      </c>
+      <c r="V36">
+        <v>1109.1600000000001</v>
+      </c>
+      <c r="W36">
+        <v>1145.02</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z36">
+        <v>0.01</v>
+      </c>
+      <c r="AA36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB36">
+        <v>0.12</v>
+      </c>
+      <c r="AC36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD36">
+        <v>1.01</v>
+      </c>
+      <c r="AE36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF36">
+        <v>10.51</v>
+      </c>
+      <c r="AG36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH36">
+        <v>126.6</v>
+      </c>
+      <c r="AI36" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>0.06</v>
+      </c>
+      <c r="C37">
+        <v>0.06</v>
+      </c>
+      <c r="D37">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E37">
+        <v>0.67</v>
+      </c>
+      <c r="F37">
+        <v>5.46</v>
+      </c>
+      <c r="G37">
+        <v>5.95</v>
+      </c>
+      <c r="H37">
+        <v>54.15</v>
+      </c>
+      <c r="I37">
+        <v>54.63</v>
+      </c>
+      <c r="J37">
+        <v>597.88</v>
+      </c>
+      <c r="K37">
+        <v>603.29</v>
+      </c>
+      <c r="M37" t="s">
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <v>0.49</v>
+      </c>
+      <c r="O37">
+        <v>0.51</v>
+      </c>
+      <c r="P37">
+        <v>3.54</v>
+      </c>
+      <c r="Q37">
+        <v>3.91</v>
+      </c>
+      <c r="R37">
+        <v>34.97</v>
+      </c>
+      <c r="S37">
+        <v>33.75</v>
+      </c>
+      <c r="T37">
+        <v>326.54000000000002</v>
+      </c>
+      <c r="U37">
+        <v>332.89</v>
+      </c>
+      <c r="V37">
+        <v>3797.66</v>
+      </c>
+      <c r="W37">
+        <v>3719.32</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z37">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AA37">
+        <v>0.01</v>
+      </c>
+      <c r="AB37">
+        <v>0.09</v>
+      </c>
+      <c r="AC37">
+        <v>0.09</v>
+      </c>
+      <c r="AD37">
+        <v>0.96</v>
+      </c>
+      <c r="AE37">
+        <v>0.86</v>
+      </c>
+      <c r="AF37">
+        <v>9.32</v>
+      </c>
+      <c r="AG37">
+        <v>8.61</v>
+      </c>
+      <c r="AH37">
+        <v>117.4</v>
+      </c>
+      <c r="AI37">
+        <v>97.46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>0.08</v>
+      </c>
+      <c r="C38">
+        <v>0.06</v>
+      </c>
+      <c r="D38">
+        <v>0.54</v>
+      </c>
+      <c r="E38">
+        <v>0.52</v>
+      </c>
+      <c r="F38">
+        <v>4.99</v>
+      </c>
+      <c r="G38">
+        <v>4.74</v>
+      </c>
+      <c r="H38">
+        <v>50.16</v>
+      </c>
+      <c r="I38">
+        <v>48.12</v>
+      </c>
+      <c r="J38">
+        <v>526.04</v>
+      </c>
+      <c r="K38">
+        <v>534.75</v>
+      </c>
+      <c r="M38" t="s">
+        <v>7</v>
+      </c>
+      <c r="N38">
+        <v>0.22</v>
+      </c>
+      <c r="O38">
+        <v>0.19</v>
+      </c>
+      <c r="P38">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="Q38">
+        <v>2.48</v>
+      </c>
+      <c r="R38">
+        <v>31.44</v>
+      </c>
+      <c r="S38">
+        <v>30.7</v>
+      </c>
+      <c r="T38">
+        <v>373.79</v>
+      </c>
+      <c r="U38">
+        <v>372.68</v>
+      </c>
+      <c r="V38">
+        <v>4903.08</v>
+      </c>
+      <c r="W38">
+        <v>4873.07</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z38">
+        <v>0.01</v>
+      </c>
+      <c r="AA38" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC38">
+        <v>0.52</v>
+      </c>
+      <c r="AD38">
+        <v>0.68</v>
+      </c>
+      <c r="AE38">
+        <v>4.74</v>
+      </c>
+      <c r="AF38">
+        <v>6.91</v>
+      </c>
+      <c r="AG38">
+        <v>48.12</v>
+      </c>
+      <c r="AH38">
+        <v>103.77</v>
+      </c>
+      <c r="AI38">
+        <v>534.75</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="29">
+    <mergeCell ref="Y32:AI32"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="AF34:AG34"/>
+    <mergeCell ref="AH34:AI34"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="M32:W32"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="T34:U34"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A13:U13"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="H15:M15"/>
     <mergeCell ref="O15:T15"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="H23:M23"/>
     <mergeCell ref="O23:T23"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A13:U13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed strat2 vector tests
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="17">
   <si>
     <t>10^3</t>
   </si>
@@ -120,13 +120,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,55 +429,55 @@
       <c r="B1" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="H5" s="4" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="O5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -695,55 +695,55 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="H15" s="4" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="H15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="O15" s="4" t="s">
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="O15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
@@ -835,17 +835,17 @@
       <c r="P18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>13</v>
+      <c r="Q18" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="S18" s="3">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="T18" s="3">
+        <v>54.75</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
@@ -961,30 +961,30 @@
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="H23" s="4" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="H23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="O23" s="4" t="s">
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="O23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
@@ -1053,7 +1053,7 @@
         <v>507.99</v>
       </c>
       <c r="H26" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I26">
         <v>0.13</v>
@@ -1071,7 +1071,7 @@
         <v>1109.1600000000001</v>
       </c>
       <c r="O26" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="P26">
         <v>0.01</v>
@@ -1109,7 +1109,7 @@
         <v>511.5</v>
       </c>
       <c r="H27" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I27">
         <v>0.13</v>
@@ -1127,22 +1127,22 @@
         <v>1145.02</v>
       </c>
       <c r="O27" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="P27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>13</v>
+      <c r="Q27" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="R27" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="S27" s="3">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="T27" s="3">
+        <v>54.75</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
@@ -1202,200 +1202,200 @@
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="M32" s="4" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="M32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="Y32" s="4" t="s">
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="Y32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
-      <c r="AD32" s="4"/>
-      <c r="AE32" s="5"/>
-      <c r="AF32" s="5"/>
-      <c r="AG32" s="5"/>
-      <c r="AH32" s="5"/>
-      <c r="AI32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="6"/>
+      <c r="AG32" s="6"/>
+      <c r="AH32" s="6"/>
+      <c r="AI32" s="6"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="6" t="s">
+      <c r="C34" s="8"/>
+      <c r="D34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="7"/>
-      <c r="J34" s="6" t="s">
+      <c r="I34" s="8"/>
+      <c r="J34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K34" s="7"/>
-      <c r="N34" s="6" t="s">
+      <c r="K34" s="8"/>
+      <c r="N34" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="O34" s="7"/>
-      <c r="P34" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S34" s="7"/>
-      <c r="T34" s="6" t="s">
+      <c r="O34" s="8"/>
+      <c r="P34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" s="8"/>
+      <c r="T34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="U34" s="7"/>
-      <c r="V34" s="6" t="s">
+      <c r="U34" s="8"/>
+      <c r="V34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="W34" s="7"/>
-      <c r="Z34" s="6" t="s">
+      <c r="W34" s="8"/>
+      <c r="Z34" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AA34" s="7"/>
-      <c r="AB34" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC34" s="7"/>
-      <c r="AD34" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE34" s="7"/>
-      <c r="AF34" s="6" t="s">
+      <c r="AA34" s="8"/>
+      <c r="AB34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="8"/>
+      <c r="AD34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="8"/>
+      <c r="AF34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AG34" s="7"/>
-      <c r="AH34" s="6" t="s">
+      <c r="AG34" s="8"/>
+      <c r="AH34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AI34" s="7"/>
+      <c r="AI34" s="8"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B35" s="8">
-        <v>1</v>
-      </c>
-      <c r="C35" s="8">
-        <v>2</v>
-      </c>
-      <c r="D35" s="8">
-        <v>1</v>
-      </c>
-      <c r="E35" s="8">
-        <v>2</v>
-      </c>
-      <c r="F35" s="8">
-        <v>1</v>
-      </c>
-      <c r="G35" s="8">
-        <v>2</v>
-      </c>
-      <c r="H35" s="8">
-        <v>1</v>
-      </c>
-      <c r="I35" s="8">
-        <v>2</v>
-      </c>
-      <c r="J35" s="8">
-        <v>1</v>
-      </c>
-      <c r="K35" s="8">
-        <v>2</v>
-      </c>
-      <c r="N35" s="8">
-        <v>1</v>
-      </c>
-      <c r="O35" s="8">
-        <v>2</v>
-      </c>
-      <c r="P35" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="8">
-        <v>2</v>
-      </c>
-      <c r="R35" s="8">
-        <v>1</v>
-      </c>
-      <c r="S35" s="8">
-        <v>2</v>
-      </c>
-      <c r="T35" s="8">
-        <v>1</v>
-      </c>
-      <c r="U35" s="8">
-        <v>2</v>
-      </c>
-      <c r="V35" s="8">
-        <v>1</v>
-      </c>
-      <c r="W35" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z35" s="8">
-        <v>1</v>
-      </c>
-      <c r="AA35" s="8">
-        <v>2</v>
-      </c>
-      <c r="AB35" s="8">
-        <v>1</v>
-      </c>
-      <c r="AC35" s="8">
-        <v>2</v>
-      </c>
-      <c r="AD35" s="8">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="8">
-        <v>2</v>
-      </c>
-      <c r="AF35" s="8">
-        <v>1</v>
-      </c>
-      <c r="AG35" s="8">
-        <v>2</v>
-      </c>
-      <c r="AH35" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI35" s="8">
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4">
+        <v>2</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1</v>
+      </c>
+      <c r="I35" s="4">
+        <v>2</v>
+      </c>
+      <c r="J35" s="4">
+        <v>1</v>
+      </c>
+      <c r="K35" s="4">
+        <v>2</v>
+      </c>
+      <c r="N35" s="4">
+        <v>1</v>
+      </c>
+      <c r="O35" s="4">
+        <v>2</v>
+      </c>
+      <c r="P35" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>2</v>
+      </c>
+      <c r="R35" s="4">
+        <v>1</v>
+      </c>
+      <c r="S35" s="4">
+        <v>2</v>
+      </c>
+      <c r="T35" s="4">
+        <v>1</v>
+      </c>
+      <c r="U35" s="4">
+        <v>2</v>
+      </c>
+      <c r="V35" s="4">
+        <v>1</v>
+      </c>
+      <c r="W35" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="4">
+        <v>2</v>
+      </c>
+      <c r="AF35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="4">
         <v>2</v>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="Y32:AI32"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="AD34:AE34"/>
-    <mergeCell ref="AF34:AG34"/>
-    <mergeCell ref="AH34:AI34"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="O15:T15"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="O23:T23"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A13:U13"/>
     <mergeCell ref="A32:K32"/>
     <mergeCell ref="M32:W32"/>
     <mergeCell ref="N34:O34"/>
@@ -1722,17 +1722,17 @@
     <mergeCell ref="R34:S34"/>
     <mergeCell ref="T34:U34"/>
     <mergeCell ref="V34:W34"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A13:U13"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="O15:T15"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="O23:T23"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="Y32:AI32"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="AF34:AG34"/>
+    <mergeCell ref="AH34:AI34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new tests to excel
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlada\Documents\Git\VU ISI\OP\vu-isi-student-results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlada\Documents\Git\VU ISI\OP\vu-isi-student-results-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="20">
   <si>
     <t>10^3</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>vector (2)</t>
+  </si>
+  <si>
+    <t>Class vs Struct</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>struct</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -122,6 +131,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -412,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI38"/>
+  <dimension ref="A1:AI49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,55 +442,55 @@
       <c r="B1" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="H5" s="5" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="O5" s="5" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="O5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -695,55 +708,55 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="H15" s="5" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="O15" s="5" t="s">
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="O15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
@@ -961,30 +974,30 @@
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="H23" s="5" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="H23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="O23" s="5" t="s">
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="O23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
@@ -1202,110 +1215,110 @@
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="M32" s="5" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="M32" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="Y32" s="5" t="s">
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="Y32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
-      <c r="AB32" s="5"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
-      <c r="AE32" s="6"/>
-      <c r="AF32" s="6"/>
-      <c r="AG32" s="6"/>
-      <c r="AH32" s="6"/>
-      <c r="AI32" s="6"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7"/>
+      <c r="AE32" s="8"/>
+      <c r="AF32" s="8"/>
+      <c r="AG32" s="8"/>
+      <c r="AH32" s="8"/>
+      <c r="AI32" s="8"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="7" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="10"/>
+      <c r="H34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="8"/>
-      <c r="J34" s="7" t="s">
+      <c r="I34" s="10"/>
+      <c r="J34" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K34" s="8"/>
-      <c r="N34" s="7" t="s">
+      <c r="K34" s="10"/>
+      <c r="N34" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O34" s="8"/>
-      <c r="P34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="S34" s="8"/>
-      <c r="T34" s="7" t="s">
+      <c r="O34" s="10"/>
+      <c r="P34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" s="10"/>
+      <c r="T34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="U34" s="8"/>
-      <c r="V34" s="7" t="s">
+      <c r="U34" s="10"/>
+      <c r="V34" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="W34" s="8"/>
-      <c r="Z34" s="7" t="s">
+      <c r="W34" s="10"/>
+      <c r="Z34" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC34" s="8"/>
-      <c r="AD34" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE34" s="8"/>
-      <c r="AF34" s="7" t="s">
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="10"/>
+      <c r="AD34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="10"/>
+      <c r="AF34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AG34" s="8"/>
-      <c r="AH34" s="7" t="s">
+      <c r="AG34" s="10"/>
+      <c r="AH34" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AI34" s="8"/>
+      <c r="AI34" s="10"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
@@ -1702,19 +1715,114 @@
         <v>534.75</v>
       </c>
     </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>2</v>
+      </c>
+      <c r="G47" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" t="s">
+        <v>2</v>
+      </c>
+      <c r="K47" t="s">
+        <v>3</v>
+      </c>
+      <c r="P47" s="1"/>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="O15:T15"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="O23:T23"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A13:U13"/>
+  <mergeCells count="33">
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="Y32:AI32"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="AF34:AG34"/>
+    <mergeCell ref="AH34:AI34"/>
     <mergeCell ref="A32:K32"/>
     <mergeCell ref="M32:W32"/>
     <mergeCell ref="N34:O34"/>
@@ -1727,12 +1835,17 @@
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="J34:K34"/>
-    <mergeCell ref="Y32:AI32"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="AD34:AE34"/>
-    <mergeCell ref="AF34:AG34"/>
-    <mergeCell ref="AH34:AI34"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A13:U13"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="O15:T15"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="O23:T23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Excel test file
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="27">
   <si>
     <t>10^3</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>struct</t>
+  </si>
+  <si>
+    <t>Optimization flags</t>
+  </si>
+  <si>
+    <t>class(O1)</t>
+  </si>
+  <si>
+    <t>class(O2)</t>
+  </si>
+  <si>
+    <t>class(OX)</t>
+  </si>
+  <si>
+    <t>struct(O1)</t>
+  </si>
+  <si>
+    <t>struct(O2)</t>
+  </si>
+  <si>
+    <t>struct(OX)</t>
   </si>
 </sst>
 </file>
@@ -119,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -135,6 +156,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI49"/>
+  <dimension ref="A1:AI68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:K32"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,55 +466,55 @@
       <c r="B1" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="O5" s="7" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="O5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -708,55 +732,55 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="H15" s="7" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="H15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="O15" s="7" t="s">
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="O15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
@@ -974,30 +998,30 @@
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="H23" s="7" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="H23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="O23" s="7" t="s">
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="O23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
@@ -1215,110 +1239,110 @@
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="M32" s="7" t="s">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="M32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="Y32" s="7" t="s">
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="Y32" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="7"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="8"/>
-      <c r="AF32" s="8"/>
-      <c r="AG32" s="8"/>
-      <c r="AH32" s="8"/>
-      <c r="AI32" s="8"/>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="8"/>
+      <c r="AB32" s="8"/>
+      <c r="AC32" s="8"/>
+      <c r="AD32" s="8"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
+      <c r="AI32" s="9"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="9" t="s">
+      <c r="C34" s="11"/>
+      <c r="D34" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="H34" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I34" s="10"/>
-      <c r="J34" s="9" t="s">
+      <c r="I34" s="11"/>
+      <c r="J34" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K34" s="10"/>
-      <c r="N34" s="9" t="s">
+      <c r="K34" s="11"/>
+      <c r="N34" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O34" s="10"/>
-      <c r="P34" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="S34" s="10"/>
-      <c r="T34" s="9" t="s">
+      <c r="O34" s="11"/>
+      <c r="P34" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" s="11"/>
+      <c r="T34" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="U34" s="10"/>
-      <c r="V34" s="9" t="s">
+      <c r="U34" s="11"/>
+      <c r="V34" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="W34" s="10"/>
-      <c r="Z34" s="9" t="s">
+      <c r="W34" s="11"/>
+      <c r="Z34" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="AA34" s="10"/>
-      <c r="AB34" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC34" s="10"/>
-      <c r="AD34" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE34" s="10"/>
-      <c r="AF34" s="9" t="s">
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="11"/>
+      <c r="AF34" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AG34" s="10"/>
-      <c r="AH34" s="9" t="s">
+      <c r="AG34" s="11"/>
+      <c r="AH34" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AI34" s="10"/>
+      <c r="AI34" s="11"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
@@ -1716,19 +1740,19 @@
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -1741,23 +1765,23 @@
       <c r="U43" s="5"/>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
+      <c r="E45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
+      <c r="I45" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
       <c r="L45" s="5"/>
       <c r="M45" s="5"/>
       <c r="N45" s="6"/>
@@ -1793,26 +1817,411 @@
       <c r="A48" t="s">
         <v>18</v>
       </c>
+      <c r="B48">
+        <v>2.82</v>
+      </c>
+      <c r="C48">
+        <v>28.27</v>
+      </c>
       <c r="E48" t="s">
         <v>18</v>
       </c>
+      <c r="F48">
+        <v>0.75</v>
+      </c>
+      <c r="G48">
+        <v>7.65</v>
+      </c>
       <c r="I48" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K48">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>19</v>
       </c>
+      <c r="B49">
+        <v>2.6</v>
+      </c>
+      <c r="C49">
+        <v>26.58</v>
+      </c>
       <c r="E49" t="s">
         <v>19</v>
       </c>
+      <c r="F49">
+        <v>5.08</v>
+      </c>
+      <c r="G49">
+        <v>53.29</v>
+      </c>
       <c r="I49" t="s">
         <v>19</v>
       </c>
+      <c r="J49">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K49">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" t="s">
+        <v>2</v>
+      </c>
+      <c r="K56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57">
+        <v>2.82</v>
+      </c>
+      <c r="C57">
+        <v>28.27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57">
+        <v>0.75</v>
+      </c>
+      <c r="G57">
+        <v>7.65</v>
+      </c>
+      <c r="I57" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K57">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C58">
+        <v>20.18</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58">
+        <v>0.45</v>
+      </c>
+      <c r="G58">
+        <v>4.88</v>
+      </c>
+      <c r="I58" t="s">
+        <v>21</v>
+      </c>
+      <c r="J58">
+        <v>0.2</v>
+      </c>
+      <c r="K58">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C59">
+        <v>19.98</v>
+      </c>
+      <c r="E59" t="s">
+        <v>22</v>
+      </c>
+      <c r="F59">
+        <v>0.41</v>
+      </c>
+      <c r="G59">
+        <v>4.46</v>
+      </c>
+      <c r="I59" t="s">
+        <v>22</v>
+      </c>
+      <c r="J59">
+        <v>0.19</v>
+      </c>
+      <c r="K59">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60">
+        <v>1.99</v>
+      </c>
+      <c r="C60">
+        <v>20.02</v>
+      </c>
+      <c r="E60" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60">
+        <v>0.42</v>
+      </c>
+      <c r="G60">
+        <v>4.46</v>
+      </c>
+      <c r="I60" t="s">
+        <v>23</v>
+      </c>
+      <c r="J60">
+        <v>0.19</v>
+      </c>
+      <c r="K60">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" t="s">
+        <v>2</v>
+      </c>
+      <c r="G64" t="s">
+        <v>3</v>
+      </c>
+      <c r="J64" t="s">
+        <v>2</v>
+      </c>
+      <c r="K64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65">
+        <v>2.6</v>
+      </c>
+      <c r="C65">
+        <v>26.58</v>
+      </c>
+      <c r="E65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65">
+        <v>5.08</v>
+      </c>
+      <c r="G65">
+        <v>53.29</v>
+      </c>
+      <c r="I65" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K65">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C66">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="E66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66">
+        <v>3.13</v>
+      </c>
+      <c r="G66">
+        <v>32.69</v>
+      </c>
+      <c r="I66" t="s">
+        <v>24</v>
+      </c>
+      <c r="J66">
+        <v>0.2</v>
+      </c>
+      <c r="K66">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67">
+        <v>1.93</v>
+      </c>
+      <c r="C67">
+        <v>19.11</v>
+      </c>
+      <c r="E67" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67">
+        <v>3.09</v>
+      </c>
+      <c r="G67">
+        <v>29.28</v>
+      </c>
+      <c r="I67" t="s">
+        <v>25</v>
+      </c>
+      <c r="J67">
+        <v>0.19</v>
+      </c>
+      <c r="K67">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68">
+        <v>1.93</v>
+      </c>
+      <c r="C68">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="E68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68">
+        <v>3.05</v>
+      </c>
+      <c r="G68">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="I68" t="s">
+        <v>26</v>
+      </c>
+      <c r="J68">
+        <v>0.2</v>
+      </c>
+      <c r="K68">
+        <v>1.62</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="40">
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="O15:T15"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="O23:T23"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A13:U13"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="E45:G45"/>
     <mergeCell ref="I45:K45"/>
@@ -1829,23 +2238,6 @@
     <mergeCell ref="P34:Q34"/>
     <mergeCell ref="R34:S34"/>
     <mergeCell ref="T34:U34"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A13:U13"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="O15:T15"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="O23:T23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>